<commit_message>
Canada - removed Release #
</commit_message>
<xml_diff>
--- a/blueprint-jira-better-excel/Canada-Issues.xlsx
+++ b/blueprint-jira-better-excel/Canada-Issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\etc\blueprint-jira-better-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0F789F-DDC0-4A51-8EA7-F71EFC75EC06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59444C68-D2B7-42EF-81C9-5B81AB359FCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="688" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="199">
   <si>
     <t>Status</t>
   </si>
@@ -1279,19 +1279,7 @@
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1301,6 +1289,24 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1327,7 +1333,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex Folomechine" refreshedDate="44348.719207175927" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="60" xr:uid="{00000000-000A-0000-FFFF-FFFF13000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex Folomechine" refreshedDate="44348.721334027781" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="60" xr:uid="{00000000-000A-0000-FFFF-FFFF13000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="issues"/>
   </cacheSource>
@@ -4414,7 +4420,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
-  <location ref="A6:C7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <location ref="A5:C6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="50">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
     <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
@@ -4546,7 +4552,7 @@
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
+    <pivotField showAll="0">
       <items count="5">
         <item x="0"/>
         <item x="1"/>
@@ -4586,10 +4592,9 @@
       <x v="1"/>
     </i>
   </colItems>
-  <pageFields count="3">
+  <pageFields count="2">
     <pageField fld="30" hier="-1"/>
     <pageField fld="1" hier="-1"/>
-    <pageField fld="39" item="2" hier="-1"/>
   </pageFields>
   <dataFields count="2">
     <dataField name="Bug Count" fld="0" subtotal="count" baseField="0" baseItem="0"/>
@@ -4609,7 +4614,7 @@
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{47FAF9B3-F1B1-4B18-B603-59ADFB7917AB}" name="PivotTable4" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A6:F10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
+  <location ref="A5:F9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="50">
     <pivotField showAll="0"/>
     <pivotField name="To" axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -4746,7 +4751,7 @@
       </items>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
+    <pivotField showAll="0">
       <items count="5">
         <item x="0"/>
         <item x="1"/>
@@ -4822,11 +4827,10 @@
       <x v="4"/>
     </i>
   </colItems>
-  <pageFields count="4">
+  <pageFields count="3">
     <pageField fld="1" hier="-1"/>
     <pageField fld="37" item="1" hier="-1"/>
     <pageField fld="30" item="3" hier="-1"/>
-    <pageField fld="39" item="2" hier="-1"/>
   </pageFields>
   <dataFields count="5">
     <dataField name="Total Estimate" fld="13" baseField="10" baseItem="1"/>
@@ -4849,7 +4853,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="4">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2" selected="0">
@@ -5272,15 +5276,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
@@ -5308,31 +5312,23 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="B4" s="17">
-        <v>12.2</v>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" t="s">
-        <v>118</v>
-      </c>
-      <c r="C6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
+      <c r="A6" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5341,10 +5337,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF66290E-43B2-4D8C-B12D-4C7A8A7BDD6A}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5381,37 +5377,45 @@
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="B4" s="17">
-        <v>12.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B5" s="30" t="s">
         <v>162</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C5" s="30" t="s">
         <v>180</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D5" s="30" t="s">
         <v>179</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E5" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F5" s="30" t="s">
         <v>163</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="B6" s="20">
+        <v>5</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="29">
+        <v>0</v>
+      </c>
+      <c r="F6" s="29">
+        <v>1</v>
+      </c>
+    </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
-        <v>194</v>
+      <c r="A7" s="32" t="s">
+        <v>192</v>
       </c>
       <c r="B7" s="20">
         <v>5</v>
@@ -5426,8 +5430,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="32" t="s">
-        <v>192</v>
+      <c r="A8" s="23" t="s">
+        <v>84</v>
       </c>
       <c r="B8" s="20">
         <v>5</v>
@@ -5442,8 +5446,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="23" t="s">
-        <v>84</v>
+      <c r="A9" s="17" t="s">
+        <v>50</v>
       </c>
       <c r="B9" s="20">
         <v>5</v>
@@ -5457,25 +5461,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="20">
-        <v>5</v>
-      </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="29">
-        <v>0</v>
-      </c>
-      <c r="F10" s="29">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting pivot="1" sqref="B8">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+  <conditionalFormatting pivot="1" sqref="B7">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>